<commit_message>
adds full alphabet, numbers and colon to letters
</commit_message>
<xml_diff>
--- a/alphabetJSONCreator.xlsx
+++ b/alphabetJSONCreator.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>.</t>
   </si>
@@ -59,10 +59,13 @@
     <t>{offsetx:2,offsety:2},</t>
   </si>
   <si>
-    <t>{offsetx:2,offsety:3},</t>
-  </si>
-  <si>
     <t>{offsetx:2,offsety:4},</t>
+  </si>
+  <si>
+    <t>{offsetx:0,offsety:3},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -189,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +518,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q15"/>
+      <selection activeCell="K1" sqref="K1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,14 +542,16 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="K2" t="str">
         <f>IF(A2=".","{offsetx:0,offsety:2},","")</f>
-        <v>{offsetx:0,offsety:2},</v>
+        <v/>
       </c>
       <c r="Q2" t="s">
         <v>3</v>
@@ -571,7 +577,9 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
@@ -580,7 +588,7 @@
         <v/>
       </c>
       <c r="Q4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -658,7 +666,7 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K12" t="str">
         <f>IF(C2=".","{offsetx:2,offsety:1},","")</f>
-        <v/>
+        <v>{offsetx:2,offsety:1},</v>
       </c>
       <c r="Q12" t="s">
         <v>1</v>
@@ -679,7 +687,7 @@
         <v>{offsetx:2,offsety:3},</v>
       </c>
       <c r="Q14" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -688,7 +696,7 @@
         <v>{offsetx:2,offsety:4},</v>
       </c>
       <c r="Q15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>